<commit_message>
Further updates to tables & markdown
</commit_message>
<xml_diff>
--- a/data/human/LSR1_ROB_ME.xlsx
+++ b/data/human/LSR1_ROB_ME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennett\Documents\GitHub\LSR1_anhedonia_H\data\human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D9A728-7BDB-466E-BAB0-1CC7EDE20951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51045EA7-5326-4450-8B4C-29F948EA4F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="166">
   <si>
     <t>Meta-analysis</t>
   </si>
@@ -444,12 +444,6 @@
   </si>
   <si>
     <t>Specify n</t>
-  </si>
-  <si>
-    <t>Domain 3.Potential for missing studies across systematic review</t>
-  </si>
-  <si>
-    <t>Domain 4. Assess RoB due to missing evidence in meta-analysis</t>
   </si>
   <si>
     <t>Overall Risk of Bias Judgement</t>
@@ -549,20 +543,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -632,23 +619,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -666,43 +642,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9294BED8-1868-405F-B11C-D212EE50A2B5}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="109" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -4034,13 +3989,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6308CE74-3E75-401F-8C60-4F0410E439EC}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4053,167 +4008,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="A1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="G1" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="H1" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="I1" s="8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J1" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="K1" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="L1" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M1" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="N1" s="8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O1" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="P1" s="8">
+        <v>4.8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="11">
-        <v>3.1</v>
-      </c>
-      <c r="G2" s="11">
-        <v>3.2</v>
-      </c>
-      <c r="H2" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="I2" s="12">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J2" s="12">
-        <v>4.2</v>
-      </c>
-      <c r="K2" s="12">
-        <v>4.3</v>
-      </c>
-      <c r="L2" s="12">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M2" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="N2" s="12">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="O2" s="12">
-        <v>4.7</v>
-      </c>
-      <c r="P2" s="12">
-        <v>4.8</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="C2" t="s">
         <v>138</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>2079</v>
+      </c>
+      <c r="F2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>3517</v>
+      </c>
+      <c r="F3" t="s">
         <v>139</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>140</v>
       </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>2079</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" t="s">
         <v>141</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O3" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q3" t="s">
         <v>142</v>
-      </c>
-      <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K3" t="s">
-        <v>141</v>
-      </c>
-      <c r="L3" t="s">
-        <v>142</v>
-      </c>
-      <c r="M3" t="s">
-        <v>141</v>
-      </c>
-      <c r="N3" t="s">
-        <v>143</v>
-      </c>
-      <c r="O3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P3" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>145</v>
@@ -4222,157 +4177,157 @@
         <v>146</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="E4">
-        <v>3517</v>
+        <v>9725</v>
       </c>
       <c r="F4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" t="s">
         <v>141</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" t="s">
+        <v>141</v>
+      </c>
+      <c r="O4" t="s">
+        <v>148</v>
+      </c>
+      <c r="P4" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q4" t="s">
         <v>142</v>
-      </c>
-      <c r="H4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" t="s">
-        <v>141</v>
-      </c>
-      <c r="J4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K4" t="s">
-        <v>141</v>
-      </c>
-      <c r="L4" t="s">
-        <v>142</v>
-      </c>
-      <c r="M4" t="s">
-        <v>141</v>
-      </c>
-      <c r="N4" t="s">
-        <v>143</v>
-      </c>
-      <c r="O4" t="s">
-        <v>143</v>
-      </c>
-      <c r="P4" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>5375</v>
+      </c>
+      <c r="F5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" t="s">
+        <v>139</v>
+      </c>
+      <c r="J5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" t="s">
         <v>147</v>
       </c>
-      <c r="C5" t="s">
+      <c r="L5" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N5" t="s">
+        <v>141</v>
+      </c>
+      <c r="O5" t="s">
         <v>148</v>
       </c>
-      <c r="D5">
-        <v>52</v>
-      </c>
-      <c r="E5">
-        <v>9725</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="P5" t="s">
         <v>141</v>
       </c>
-      <c r="G5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J5" t="s">
-        <v>143</v>
-      </c>
-      <c r="K5" t="s">
-        <v>149</v>
-      </c>
-      <c r="L5" t="s">
-        <v>150</v>
-      </c>
-      <c r="M5" t="s">
-        <v>141</v>
-      </c>
-      <c r="N5" t="s">
-        <v>143</v>
-      </c>
-      <c r="O5" t="s">
-        <v>150</v>
-      </c>
-      <c r="P5" t="s">
-        <v>143</v>
-      </c>
       <c r="Q5" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="E6">
+        <v>6026</v>
+      </c>
+      <c r="F6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L6" t="s">
+        <v>140</v>
+      </c>
+      <c r="M6" t="s">
+        <v>139</v>
+      </c>
+      <c r="N6" t="s">
+        <v>141</v>
+      </c>
+      <c r="O6" t="s">
+        <v>148</v>
+      </c>
+      <c r="P6" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q6" t="s">
         <v>151</v>
-      </c>
-      <c r="C6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <v>5375</v>
-      </c>
-      <c r="F6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" t="s">
-        <v>141</v>
-      </c>
-      <c r="J6" t="s">
-        <v>143</v>
-      </c>
-      <c r="K6" t="s">
-        <v>149</v>
-      </c>
-      <c r="L6" t="s">
-        <v>142</v>
-      </c>
-      <c r="M6" t="s">
-        <v>141</v>
-      </c>
-      <c r="N6" t="s">
-        <v>143</v>
-      </c>
-      <c r="O6" t="s">
-        <v>150</v>
-      </c>
-      <c r="P6" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>154</v>
@@ -4381,51 +4336,51 @@
         <v>155</v>
       </c>
       <c r="D7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>6026</v>
+        <v>6895</v>
       </c>
       <c r="F7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J7" t="s">
         <v>141</v>
       </c>
-      <c r="G7" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" t="s">
-        <v>142</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L7" t="s">
+        <v>140</v>
+      </c>
+      <c r="M7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" t="s">
         <v>141</v>
       </c>
-      <c r="J7" t="s">
-        <v>143</v>
-      </c>
-      <c r="K7" t="s">
-        <v>149</v>
-      </c>
-      <c r="L7" t="s">
-        <v>142</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
+        <v>148</v>
+      </c>
+      <c r="P7" t="s">
         <v>141</v>
       </c>
-      <c r="N7" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" t="s">
-        <v>150</v>
-      </c>
-      <c r="P7" t="s">
-        <v>143</v>
-      </c>
       <c r="Q7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>156</v>
@@ -4434,51 +4389,51 @@
         <v>157</v>
       </c>
       <c r="D8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8">
-        <v>6895</v>
+        <v>7084</v>
       </c>
       <c r="F8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" t="s">
         <v>141</v>
       </c>
-      <c r="G8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
+        <v>147</v>
+      </c>
+      <c r="L8" t="s">
+        <v>140</v>
+      </c>
+      <c r="M8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N8" t="s">
         <v>141</v>
       </c>
-      <c r="J8" t="s">
-        <v>143</v>
-      </c>
-      <c r="K8" t="s">
-        <v>149</v>
-      </c>
-      <c r="L8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
+        <v>148</v>
+      </c>
+      <c r="P8" t="s">
         <v>141</v>
       </c>
-      <c r="N8" t="s">
-        <v>143</v>
-      </c>
-      <c r="O8" t="s">
-        <v>150</v>
-      </c>
-      <c r="P8" t="s">
-        <v>143</v>
-      </c>
       <c r="Q8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>158</v>
@@ -4487,51 +4442,51 @@
         <v>159</v>
       </c>
       <c r="D9">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E9">
-        <v>7084</v>
+        <v>6432</v>
       </c>
       <c r="F9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" t="s">
         <v>141</v>
       </c>
-      <c r="G9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
+        <v>147</v>
+      </c>
+      <c r="L9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" t="s">
+        <v>139</v>
+      </c>
+      <c r="N9" t="s">
         <v>141</v>
       </c>
-      <c r="J9" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" t="s">
-        <v>149</v>
-      </c>
-      <c r="L9" t="s">
-        <v>142</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
+        <v>148</v>
+      </c>
+      <c r="P9" t="s">
         <v>141</v>
       </c>
-      <c r="N9" t="s">
-        <v>143</v>
-      </c>
-      <c r="O9" t="s">
-        <v>150</v>
-      </c>
-      <c r="P9" t="s">
-        <v>143</v>
-      </c>
       <c r="Q9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>160</v>
@@ -4540,51 +4495,51 @@
         <v>161</v>
       </c>
       <c r="D10">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E10">
-        <v>6432</v>
+        <v>7046</v>
       </c>
       <c r="F10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" t="s">
+        <v>139</v>
+      </c>
+      <c r="J10" t="s">
         <v>141</v>
       </c>
-      <c r="G10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H10" t="s">
-        <v>142</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
+        <v>147</v>
+      </c>
+      <c r="L10" t="s">
+        <v>140</v>
+      </c>
+      <c r="M10" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" t="s">
         <v>141</v>
       </c>
-      <c r="J10" t="s">
-        <v>143</v>
-      </c>
-      <c r="K10" t="s">
-        <v>149</v>
-      </c>
-      <c r="L10" t="s">
-        <v>142</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
+        <v>148</v>
+      </c>
+      <c r="P10" t="s">
         <v>141</v>
       </c>
-      <c r="N10" t="s">
-        <v>143</v>
-      </c>
-      <c r="O10" t="s">
-        <v>150</v>
-      </c>
-      <c r="P10" t="s">
-        <v>143</v>
-      </c>
       <c r="Q10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>162</v>
@@ -4593,51 +4548,51 @@
         <v>163</v>
       </c>
       <c r="D11">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E11">
-        <v>7046</v>
+        <v>9030</v>
       </c>
       <c r="F11" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" t="s">
+        <v>139</v>
+      </c>
+      <c r="J11" t="s">
         <v>141</v>
       </c>
-      <c r="G11" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" t="s">
-        <v>142</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
+        <v>147</v>
+      </c>
+      <c r="L11" t="s">
+        <v>140</v>
+      </c>
+      <c r="M11" t="s">
+        <v>139</v>
+      </c>
+      <c r="N11" t="s">
         <v>141</v>
       </c>
-      <c r="J11" t="s">
-        <v>143</v>
-      </c>
-      <c r="K11" t="s">
-        <v>149</v>
-      </c>
-      <c r="L11" t="s">
-        <v>142</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
+        <v>148</v>
+      </c>
+      <c r="P11" t="s">
         <v>141</v>
       </c>
-      <c r="N11" t="s">
-        <v>143</v>
-      </c>
-      <c r="O11" t="s">
-        <v>150</v>
-      </c>
-      <c r="P11" t="s">
-        <v>143</v>
-      </c>
       <c r="Q11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>164</v>
@@ -4646,99 +4601,46 @@
         <v>165</v>
       </c>
       <c r="D12">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>9030</v>
+        <v>962</v>
       </c>
       <c r="F12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12" t="s">
+        <v>139</v>
+      </c>
+      <c r="J12" t="s">
         <v>141</v>
       </c>
-      <c r="G12" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" t="s">
-        <v>142</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
+        <v>147</v>
+      </c>
+      <c r="L12" t="s">
+        <v>140</v>
+      </c>
+      <c r="M12" t="s">
+        <v>139</v>
+      </c>
+      <c r="N12" t="s">
         <v>141</v>
       </c>
-      <c r="J12" t="s">
-        <v>143</v>
-      </c>
-      <c r="K12" t="s">
-        <v>149</v>
-      </c>
-      <c r="L12" t="s">
-        <v>142</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
+        <v>148</v>
+      </c>
+      <c r="P12" t="s">
         <v>141</v>
       </c>
-      <c r="N12" t="s">
-        <v>143</v>
-      </c>
-      <c r="O12" t="s">
-        <v>150</v>
-      </c>
-      <c r="P12" t="s">
-        <v>143</v>
-      </c>
       <c r="Q12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>962</v>
-      </c>
-      <c r="F13" t="s">
-        <v>141</v>
-      </c>
-      <c r="G13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H13" t="s">
-        <v>142</v>
-      </c>
-      <c r="I13" t="s">
-        <v>141</v>
-      </c>
-      <c r="J13" t="s">
-        <v>143</v>
-      </c>
-      <c r="K13" t="s">
-        <v>149</v>
-      </c>
-      <c r="L13" t="s">
-        <v>142</v>
-      </c>
-      <c r="M13" t="s">
-        <v>141</v>
-      </c>
-      <c r="N13" t="s">
-        <v>143</v>
-      </c>
-      <c r="O13" t="s">
-        <v>150</v>
-      </c>
-      <c r="P13" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -4756,17 +4658,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="66b5d41f-65e9-4808-95b5-49073c9d5630">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB673AF35069A14091CC370CA55BC6F9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1509bc80408706fd720711ca07d8938b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="66b5d41f-65e9-4808-95b5-49073c9d5630" xmlns:ns3="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c01dabd162878ec2c948aad2190d4e6" ns2:_="" ns3:_="">
     <xsd:import namespace="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
@@ -4989,6 +4880,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="66b5d41f-65e9-4808-95b5-49073c9d5630">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89E00C62-8D17-4E4D-92D5-A8A366EBF401}">
   <ds:schemaRefs>
@@ -4998,17 +4900,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC009D54-E67B-4F50-91A1-625F8A0F5DC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
-    <ds:schemaRef ds:uri="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFEBB03B-2B17-451A-BB14-6DCE503F9AB6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5025,4 +4916,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC009D54-E67B-4F50-91A1-625F8A0F5DC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
+    <ds:schemaRef ds:uri="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated tables to format decimals
</commit_message>
<xml_diff>
--- a/data/human/LSR1_ROB_ME.xlsx
+++ b/data/human/LSR1_ROB_ME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennett\Documents\GitHub\LSR1_anhedonia_H\data\human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51045EA7-5326-4450-8B4C-29F948EA4F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C3C67-5634-40E1-A9B2-44E383C9378F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="177">
   <si>
     <t>Meta-analysis</t>
   </si>
@@ -534,6 +534,39 @@
   </si>
   <si>
     <t>OR 1.90 95%CI 1.13, 3.19</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.8</t>
   </si>
 </sst>
 </file>
@@ -656,8 +689,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3995,7 +4028,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4023,38 +4056,38 @@
       <c r="E1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="G1" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="H1" s="7">
-        <v>3.3</v>
-      </c>
-      <c r="I1" s="8">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J1" s="8">
-        <v>4.2</v>
-      </c>
-      <c r="K1" s="8">
-        <v>4.3</v>
-      </c>
-      <c r="L1" s="8">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M1" s="8">
-        <v>4.5</v>
-      </c>
-      <c r="N1" s="8">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="O1" s="8">
-        <v>4.7</v>
-      </c>
-      <c r="P1" s="8">
-        <v>4.8</v>
+      <c r="F1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>136</v>
@@ -4649,12 +4682,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="66b5d41f-65e9-4808-95b5-49073c9d5630">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4881,20 +4916,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="66b5d41f-65e9-4808-95b5-49073c9d5630">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89E00C62-8D17-4E4D-92D5-A8A366EBF401}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC009D54-E67B-4F50-91A1-625F8A0F5DC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
+    <ds:schemaRef ds:uri="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4919,12 +4955,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC009D54-E67B-4F50-91A1-625F8A0F5DC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89E00C62-8D17-4E4D-92D5-A8A366EBF401}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66b5d41f-65e9-4808-95b5-49073c9d5630"/>
-    <ds:schemaRef ds:uri="f7f8f54e-e19b-4cd3-934a-81b57a2c13ba"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>